<commit_message>
adjusted files for MOBILITIES case
</commit_message>
<xml_diff>
--- a/Shocks/ShockMap.xlsx
+++ b/Shocks/ShockMap.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\FULFILL\Github Code\Shocks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lorenzorinaldi/Documents/GitHub/SESAM/FULFILL_MARIO/Shocks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C73D1941-B38E-420D-AA2B-9F53CDD3A49C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5843A5A5-CFF4-1F43-92D0-7605E362CF21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B1A9D9D1-B9A4-46DF-A7E5-B87F17987466}"/>
+    <workbookView xWindow="-9240" yWindow="-28800" windowWidth="51200" windowHeight="28800" xr2:uid="{B1A9D9D1-B9A4-46DF-A7E5-B87F17987466}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="81">
   <si>
     <t>REF</t>
   </si>
@@ -273,6 +273,15 @@
   </si>
   <si>
     <t>vkm pc B</t>
+  </si>
+  <si>
+    <t>car_mix NZE_MOB</t>
+  </si>
+  <si>
+    <t>MOB</t>
+  </si>
+  <si>
+    <t>vkm pc MOB</t>
   </si>
 </sst>
 </file>
@@ -309,12 +318,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -329,7 +344,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -349,9 +364,21 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -367,7 +394,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -683,28 +710,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A1E1717-C5DB-4F43-964B-F0B49A8D9BEC}">
-  <dimension ref="A1:V20"/>
+  <dimension ref="A1:W20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="93" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="6" ySplit="3" topLeftCell="G4" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="177" zoomScaleNormal="130" workbookViewId="0">
+      <pane xSplit="6" ySplit="3" topLeftCell="L4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="M15" sqref="M15"/>
+      <selection pane="bottomRight" activeCell="W13" sqref="W13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.5703125" style="1" customWidth="1"/>
-    <col min="7" max="22" width="10.5703125" style="1" customWidth="1"/>
-    <col min="23" max="16384" width="9.140625" style="1"/>
+    <col min="6" max="6" width="25.5" style="1" customWidth="1"/>
+    <col min="7" max="14" width="10.5" style="1" customWidth="1"/>
+    <col min="15" max="15" width="10.5" style="7" customWidth="1"/>
+    <col min="16" max="22" width="10.5" style="1" customWidth="1"/>
+    <col min="23" max="23" width="11.6640625" style="7" customWidth="1"/>
+    <col min="24" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="F1" s="3" t="s">
         <v>17</v>
       </c>
@@ -732,7 +762,7 @@
       <c r="N1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="7" t="s">
         <v>13</v>
       </c>
       <c r="P1" s="1" t="s">
@@ -756,8 +786,11 @@
       <c r="V1" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="W1" s="7" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="F2" s="3" t="s">
         <v>18</v>
       </c>
@@ -785,7 +818,7 @@
       <c r="N2" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="O2" s="4">
+      <c r="O2" s="9">
         <v>0</v>
       </c>
       <c r="P2" s="4" t="s">
@@ -809,8 +842,11 @@
       <c r="V2" s="4" t="s">
         <v>61</v>
       </c>
+      <c r="W2" s="7" t="s">
+        <v>79</v>
+      </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>19</v>
       </c>
@@ -837,7 +873,7 @@
       <c r="L3" s="4"/>
       <c r="M3" s="4"/>
       <c r="N3" s="4"/>
-      <c r="O3" s="4"/>
+      <c r="O3" s="9"/>
       <c r="P3" s="4"/>
       <c r="Q3" s="4"/>
       <c r="R3" s="4"/>
@@ -846,7 +882,7 @@
       <c r="U3" s="4"/>
       <c r="V3" s="4"/>
     </row>
-    <row r="4" spans="1:22" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" ht="48" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -889,7 +925,7 @@
       <c r="N4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="O4" s="1" t="s">
+      <c r="O4" s="7" t="s">
         <v>27</v>
       </c>
       <c r="P4" s="1" t="s">
@@ -913,8 +949,11 @@
       <c r="V4" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="W4" s="7" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="5" spans="1:22" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -957,7 +996,7 @@
       <c r="N5" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="O5" s="1" t="s">
+      <c r="O5" s="7" t="s">
         <v>51</v>
       </c>
       <c r="P5" s="1" t="s">
@@ -981,8 +1020,11 @@
       <c r="V5" s="1" t="s">
         <v>51</v>
       </c>
+      <c r="W5" s="7" t="s">
+        <v>51</v>
+      </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -1025,7 +1067,7 @@
       <c r="N6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="O6" s="1" t="s">
+      <c r="O6" s="7" t="s">
         <v>6</v>
       </c>
       <c r="P6" s="1" t="s">
@@ -1049,76 +1091,82 @@
       <c r="V6" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="W6" s="7" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="7" spans="1:22" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:23" s="7" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A7" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="8">
         <v>4</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="G7" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H7" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="I7" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="J7" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="K7" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="L7" s="1" t="s">
+      <c r="L7" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="M7" s="1" t="s">
+      <c r="M7" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="N7" s="1" t="s">
+      <c r="N7" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="O7" s="1" t="s">
+      <c r="O7" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="P7" s="1" t="s">
+      <c r="P7" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="Q7" s="1" t="s">
+      <c r="Q7" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="R7" s="1" t="s">
+      <c r="R7" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="S7" s="1" t="s">
+      <c r="S7" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="T7" s="1" t="s">
+      <c r="T7" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="U7" s="1" t="s">
+      <c r="U7" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="V7" s="1" t="s">
+      <c r="V7" s="7" t="s">
         <v>46</v>
       </c>
+      <c r="W7" s="10" t="s">
+        <v>78</v>
+      </c>
     </row>
-    <row r="8" spans="1:22" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -1161,7 +1209,7 @@
       <c r="N8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="O8" s="1" t="s">
+      <c r="O8" s="7" t="s">
         <v>8</v>
       </c>
       <c r="P8" s="1" t="s">
@@ -1185,8 +1233,11 @@
       <c r="V8" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="W8" s="7" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="9" spans="1:22" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -1229,7 +1280,7 @@
       <c r="N9" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="O9" s="1" t="s">
+      <c r="O9" s="7" t="s">
         <v>32</v>
       </c>
       <c r="P9" s="1" t="s">
@@ -1253,8 +1304,11 @@
       <c r="V9" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="W9" s="7" t="s">
+        <v>32</v>
+      </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>39</v>
       </c>
@@ -1297,7 +1351,7 @@
       <c r="N10" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="O10" s="6" t="s">
+      <c r="O10" s="10" t="s">
         <v>30</v>
       </c>
       <c r="P10" s="6" t="s">
@@ -1321,8 +1375,11 @@
       <c r="V10" s="6" t="s">
         <v>30</v>
       </c>
+      <c r="W10" s="10" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="11" spans="1:22" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" ht="32" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -1365,7 +1422,7 @@
       <c r="N11" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="O11" s="4" t="s">
+      <c r="O11" s="9" t="s">
         <v>33</v>
       </c>
       <c r="P11" s="4" t="s">
@@ -1389,8 +1446,11 @@
       <c r="V11" s="4" t="s">
         <v>33</v>
       </c>
+      <c r="W11" s="9" t="s">
+        <v>33</v>
+      </c>
     </row>
-    <row r="12" spans="1:22" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>23</v>
       </c>
@@ -1433,7 +1493,7 @@
       <c r="N12" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="O12" s="1" t="s">
+      <c r="O12" s="7" t="s">
         <v>25</v>
       </c>
       <c r="P12" s="1" t="s">
@@ -1457,76 +1517,82 @@
       <c r="V12" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="W12" s="7" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="13" spans="1:22" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+    <row r="13" spans="1:23" s="7" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A13" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="8">
         <v>10</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E13" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="F13" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="G13" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="H13" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="I13" s="1" t="s">
+      <c r="I13" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="J13" s="1" t="s">
+      <c r="J13" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="K13" s="1" t="s">
+      <c r="K13" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="L13" s="1" t="s">
+      <c r="L13" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="M13" s="1" t="s">
+      <c r="M13" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="N13" s="1" t="s">
+      <c r="N13" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="O13" s="1" t="s">
+      <c r="O13" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="P13" s="1" t="s">
+      <c r="P13" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="Q13" s="1" t="s">
+      <c r="Q13" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="R13" s="1" t="s">
+      <c r="R13" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="S13" s="1" t="s">
+      <c r="S13" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="T13" s="1" t="s">
+      <c r="T13" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="U13" s="1" t="s">
+      <c r="U13" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="V13" s="1" t="s">
+      <c r="V13" s="7" t="s">
         <v>76</v>
       </c>
+      <c r="W13" s="10" t="s">
+        <v>80</v>
+      </c>
     </row>
-    <row r="14" spans="1:22" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -1569,7 +1635,7 @@
       <c r="N14" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="O14" s="4" t="s">
+      <c r="O14" s="9" t="s">
         <v>14</v>
       </c>
       <c r="P14" s="4" t="s">
@@ -1593,8 +1659,11 @@
       <c r="V14" s="4" t="s">
         <v>14</v>
       </c>
+      <c r="W14" s="9" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>47</v>
       </c>
@@ -1637,7 +1706,7 @@
       <c r="N15" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="O15" s="1" t="s">
+      <c r="O15" s="7" t="s">
         <v>47</v>
       </c>
       <c r="P15" s="1" t="s">
@@ -1661,8 +1730,11 @@
       <c r="V15" s="1" t="s">
         <v>47</v>
       </c>
+      <c r="W15" s="7" t="s">
+        <v>47</v>
+      </c>
     </row>
-    <row r="16" spans="1:22" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>53</v>
       </c>
@@ -1705,7 +1777,7 @@
       <c r="N16" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="O16" s="1" t="s">
+      <c r="O16" s="7" t="s">
         <v>54</v>
       </c>
       <c r="P16" s="1" t="s">
@@ -1729,8 +1801,11 @@
       <c r="V16" s="1" t="s">
         <v>54</v>
       </c>
+      <c r="W16" s="7" t="s">
+        <v>54</v>
+      </c>
     </row>
-    <row r="17" spans="1:22" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>73</v>
       </c>
@@ -1773,7 +1848,7 @@
       <c r="N17" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="O17" s="1" t="s">
+      <c r="O17" s="7" t="s">
         <v>58</v>
       </c>
       <c r="P17" s="1" t="s">
@@ -1797,8 +1872,11 @@
       <c r="V17" s="1" t="s">
         <v>58</v>
       </c>
+      <c r="W17" s="7" t="s">
+        <v>58</v>
+      </c>
     </row>
-    <row r="18" spans="1:22" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:23" ht="32" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>74</v>
       </c>
@@ -1841,7 +1919,7 @@
       <c r="N18" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="O18" s="1" t="s">
+      <c r="O18" s="7" t="s">
         <v>58</v>
       </c>
       <c r="P18" s="1" t="s">
@@ -1865,8 +1943,11 @@
       <c r="V18" s="1" t="s">
         <v>58</v>
       </c>
+      <c r="W18" s="7" t="s">
+        <v>58</v>
+      </c>
     </row>
-    <row r="19" spans="1:22" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:23" ht="32" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>62</v>
       </c>
@@ -1909,7 +1990,7 @@
       <c r="N19" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="O19" s="1" t="s">
+      <c r="O19" s="7" t="s">
         <v>63</v>
       </c>
       <c r="P19" s="1" t="s">
@@ -1933,8 +2014,11 @@
       <c r="V19" s="1" t="s">
         <v>64</v>
       </c>
+      <c r="W19" s="7" t="s">
+        <v>63</v>
+      </c>
     </row>
-    <row r="20" spans="1:22" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:23" ht="32" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>66</v>
       </c>
@@ -1977,7 +2061,7 @@
       <c r="N20" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="O20" s="1" t="s">
+      <c r="O20" s="7" t="s">
         <v>67</v>
       </c>
       <c r="P20" s="1" t="s">
@@ -2000,6 +2084,9 @@
       </c>
       <c r="V20" s="1" t="s">
         <v>68</v>
+      </c>
+      <c r="W20" s="7" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating sharing spaces and moderate car sizing BAU
We noticed that sharing spaces an moderate car sizing could be modelled more consistently in the BAU. This impacts also measure 0 and All.

New shocks are added.
</commit_message>
<xml_diff>
--- a/Shocks/ShockMap.xlsx
+++ b/Shocks/ShockMap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/14a790445df90286/Documenti/GitHub/FULFILL_MARIO/Shocks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="44" documentId="13_ncr:1_{5843A5A5-CFF4-1F43-92D0-7605E362CF21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2985CA44-E8D0-4E87-9224-ED317D26FCBD}"/>
+  <xr:revisionPtr revIDLastSave="52" documentId="13_ncr:1_{5843A5A5-CFF4-1F43-92D0-7605E362CF21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6E3A4CA0-CC91-4ED5-A2C7-F7FE92F7E44B}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{B1A9D9D1-B9A4-46DF-A7E5-B87F17987466}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="87">
   <si>
     <t>REF</t>
   </si>
@@ -281,12 +281,6 @@
     <t>BAU</t>
   </si>
   <si>
-    <t>car-eff BAU - clustering</t>
-  </si>
-  <si>
-    <t>car-eff BAU-M - clustering</t>
-  </si>
-  <si>
     <t>hs-eff BAU</t>
   </si>
   <si>
@@ -306,18 +300,6 @@
   </si>
   <si>
     <t>hs-mix BAU - clustering</t>
-  </si>
-  <si>
-    <t>m2pc BAU</t>
-  </si>
-  <si>
-    <t>m2pc BAU-S</t>
-  </si>
-  <si>
-    <t>car-emi BAU - clustering</t>
-  </si>
-  <si>
-    <t>car-emi BAU-M - clustering</t>
   </si>
 </sst>
 </file>
@@ -749,10 +731,10 @@
   <dimension ref="A1:AE20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="6" ySplit="3" topLeftCell="N4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="3" topLeftCell="O4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="T12" sqref="T12"/>
+      <selection pane="bottomRight" activeCell="AE1" activeCellId="1" sqref="Y1:Y1048576 AE1:AE1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1061,7 +1043,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:31" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:31" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1132,28 +1114,28 @@
         <v>49</v>
       </c>
       <c r="X5" s="1" t="s">
-        <v>80</v>
+        <v>49</v>
       </c>
       <c r="Y5" s="1" t="s">
-        <v>81</v>
+        <v>50</v>
       </c>
       <c r="Z5" s="1" t="s">
-        <v>80</v>
+        <v>49</v>
       </c>
       <c r="AA5" s="1" t="s">
-        <v>80</v>
+        <v>49</v>
       </c>
       <c r="AB5" s="1" t="s">
-        <v>81</v>
+        <v>50</v>
       </c>
       <c r="AC5" s="1" t="s">
-        <v>80</v>
+        <v>49</v>
       </c>
       <c r="AD5" s="1" t="s">
-        <v>80</v>
+        <v>49</v>
       </c>
       <c r="AE5" s="1" t="s">
-        <v>80</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:31" ht="28.8" x14ac:dyDescent="0.3">
@@ -1227,28 +1209,28 @@
         <v>6</v>
       </c>
       <c r="X6" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="Y6" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="Z6" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="AA6" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="AB6" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="AC6" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="AD6" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="AE6" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:31" s="7" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -1322,28 +1304,28 @@
         <v>76</v>
       </c>
       <c r="X7" s="7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="Y7" s="7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="Z7" s="7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="AA7" s="7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="AB7" s="7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="AC7" s="7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="AD7" s="7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="AE7" s="7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:31" ht="28.8" x14ac:dyDescent="0.3">
@@ -1417,28 +1399,28 @@
         <v>8</v>
       </c>
       <c r="X8" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="Y8" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="Z8" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="AA8" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="AB8" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="AC8" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="AD8" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="AE8" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:31" ht="43.2" x14ac:dyDescent="0.3">
@@ -1461,79 +1443,79 @@
         <v>41</v>
       </c>
       <c r="G9" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="O9" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="R9" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="S9" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="T9" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="U9" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="V9" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="W9" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="X9" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="Y9" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="Z9" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="J9" s="1" t="s">
+      <c r="AA9" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="K9" s="1" t="s">
+      <c r="AB9" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="L9" s="1" t="s">
+      <c r="AC9" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="M9" s="1" t="s">
+      <c r="AD9" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="N9" s="1" t="s">
+      <c r="AE9" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="O9" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="P9" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="Q9" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="R9" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="S9" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="T9" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="U9" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="V9" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="W9" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="X9" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="Y9" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="Z9" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="AA9" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="AB9" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="AC9" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="AD9" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="AE9" s="1" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.3">
@@ -1702,28 +1684,28 @@
         <v>31</v>
       </c>
       <c r="X11" s="4" t="s">
-        <v>89</v>
+        <v>31</v>
       </c>
       <c r="Y11" s="4" t="s">
-        <v>90</v>
+        <v>32</v>
       </c>
       <c r="Z11" s="4" t="s">
-        <v>89</v>
+        <v>31</v>
       </c>
       <c r="AA11" s="4" t="s">
-        <v>90</v>
+        <v>32</v>
       </c>
       <c r="AB11" s="4" t="s">
-        <v>89</v>
+        <v>31</v>
       </c>
       <c r="AC11" s="4" t="s">
-        <v>89</v>
+        <v>31</v>
       </c>
       <c r="AD11" s="4" t="s">
-        <v>89</v>
+        <v>31</v>
       </c>
       <c r="AE11" s="4" t="s">
-        <v>89</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:31" ht="28.8" x14ac:dyDescent="0.3">
@@ -2082,28 +2064,28 @@
         <v>45</v>
       </c>
       <c r="X15" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="Y15" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="Z15" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="AA15" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="AB15" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="AC15" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="AD15" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="AE15" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:31" ht="43.2" x14ac:dyDescent="0.3">
@@ -2177,28 +2159,28 @@
         <v>52</v>
       </c>
       <c r="X16" s="1" t="s">
-        <v>91</v>
+        <v>52</v>
       </c>
       <c r="Y16" s="1" t="s">
-        <v>92</v>
+        <v>53</v>
       </c>
       <c r="Z16" s="1" t="s">
-        <v>91</v>
+        <v>52</v>
       </c>
       <c r="AA16" s="1" t="s">
-        <v>91</v>
+        <v>52</v>
       </c>
       <c r="AB16" s="1" t="s">
-        <v>92</v>
+        <v>53</v>
       </c>
       <c r="AC16" s="1" t="s">
-        <v>91</v>
+        <v>52</v>
       </c>
       <c r="AD16" s="1" t="s">
-        <v>91</v>
+        <v>52</v>
       </c>
       <c r="AE16" s="1" t="s">
-        <v>91</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:31" ht="28.8" x14ac:dyDescent="0.3">

</xml_diff>